<commit_message>
Runs, not quite right
</commit_message>
<xml_diff>
--- a/conejo/one_fictitious/formatted_data1.xlsx
+++ b/conejo/one_fictitious/formatted_data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pyComms\conejo\one_fictitious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1A6DA6-F940-4A5D-9CDD-77B956BC6C82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD5C7A-F558-4AED-B319-833F07462D77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B2B3255C-86D4-4B94-9983-7EF4502B7862}"/>
   </bookViews>
   <sheets>
     <sheet name="busses" sheetId="2" r:id="rId1"/>
@@ -3204,7 +3204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F8381-333D-427E-B2F5-663E2125B366}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4942,8 +4942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E240635E-BFDB-4BD5-AB72-96E8013830DA}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5024,7 +5024,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="K2">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="L2">
         <v>208</v>
@@ -5068,7 +5068,7 @@
         <v>0.158</v>
       </c>
       <c r="K3">
-        <v>40</v>
+        <v>500</v>
       </c>
       <c r="L3">
         <v>600</v>
@@ -5112,7 +5112,7 @@
         <v>0.155</v>
       </c>
       <c r="K4">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="L4">
         <v>600</v>
@@ -5173,6 +5173,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>